<commit_message>
Updated blog Milestone 2
</commit_message>
<xml_diff>
--- a/blog Milestone 2.xlsx
+++ b/blog Milestone 2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="10020"/>
+    <workbookView windowWidth="25600" windowHeight="12030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="140">
   <si>
     <t>Team Members</t>
   </si>
@@ -226,154 +226,193 @@
     <t>Created User repository and added user authentication feature. Updated UserLogin, UserRegistration, App.java files.</t>
   </si>
   <si>
+    <t>Update User Authentication</t>
+  </si>
+  <si>
+    <t>Update user authentication, login and registration.</t>
+  </si>
+  <si>
+    <t>User login and register add and remove user</t>
+  </si>
+  <si>
+    <t>Functionality implementation</t>
+  </si>
+  <si>
+    <t>Student Browse assets implemented along with advanced search</t>
+  </si>
+  <si>
+    <t>Browsing history Implemented</t>
+  </si>
+  <si>
+    <t>Block and unBlock user update for admin</t>
+  </si>
+  <si>
+    <t>Functionality implementation for admin</t>
+  </si>
+  <si>
+    <t>Update without togglecase</t>
+  </si>
+  <si>
+    <t>Rework on functional case without togglecase</t>
+  </si>
+  <si>
+    <t>Code Refactoring and correcting the attributes in the classes</t>
+  </si>
+  <si>
+    <t>Reviewing</t>
+  </si>
+  <si>
+    <t>Understanding the code classes with respect to class Diagram and reviewing peer's code for asset management and asset repository.</t>
+  </si>
+  <si>
+    <t>Developed an idea of which functionalities of assetmanagement and assetrepository class is to be used for implementing add and remove for book and other assets.</t>
+  </si>
+  <si>
     <t>Group Discussion</t>
   </si>
   <si>
     <t>Discussion on Class Diagram and task break down</t>
   </si>
   <si>
+    <t>addUser message suppression</t>
+  </si>
+  <si>
+    <t>Suppresses addUser message for initial usecase.</t>
+  </si>
+  <si>
+    <t>Coding for add and remove asset</t>
+  </si>
+  <si>
+    <t>Functionality developed for add and remove asset.</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Code Review</t>
+  </si>
+  <si>
+    <t>Reviewing peers code</t>
+  </si>
+  <si>
+    <t>ReCoding for add and remove book as an individual asset rather then all asset in common because of different attributes.</t>
+  </si>
+  <si>
+    <t>Fully functional add and remove book code.</t>
+  </si>
+  <si>
+    <t>Refactoring and learning</t>
+  </si>
+  <si>
+    <t>Identified and reviewed mistakes as pointed out by peer. Learned new java concept of super and implmenting that in the add and remove book</t>
+  </si>
+  <si>
+    <t>Refactored Add and Remove Book code.</t>
+  </si>
+  <si>
     <t>Discussion on the tasks</t>
   </si>
   <si>
+    <t>Disciussion Room function</t>
+  </si>
+  <si>
+    <t>Added discussion room repository</t>
+  </si>
+  <si>
+    <t>Test cases for User, blocking and userRepository</t>
+  </si>
+  <si>
+    <t>writing Junit testcases for the mentioned classes</t>
+  </si>
+  <si>
+    <t>Coding and debugging</t>
+  </si>
+  <si>
+    <t>Line edits, UI Changes, to string(), updateNews implementation</t>
+  </si>
+  <si>
+    <t>UI editing, implementation of toString() method and implementation of updateNews functionality</t>
+  </si>
+  <si>
+    <t>Added discussion room management and model.</t>
+  </si>
+  <si>
+    <t>Update Book details coding</t>
+  </si>
+  <si>
+    <t>Developing Functionality and Debugging</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Test cases Review</t>
+  </si>
+  <si>
+    <t>Implementing Admin services, view news toString()</t>
+  </si>
+  <si>
+    <t>Functionality implementation of adminServices and to string on viewNews</t>
+  </si>
+  <si>
+    <t>Developing initial test case for adding a book</t>
+  </si>
+  <si>
+    <t>Raw version of code developed for adding a book</t>
+  </si>
+  <si>
+    <t>Debugging</t>
+  </si>
+  <si>
+    <t>UI changes and Junit 4 to 5 conversions and rewriting testcases</t>
+  </si>
+  <si>
+    <t>rewrk on testcases</t>
+  </si>
+  <si>
+    <t>Presentation Room fuction</t>
+  </si>
+  <si>
+    <t>Refactored discussion roo code into presentation room code.</t>
+  </si>
+  <si>
+    <t>Developing test case for Remove book and debugging add book test case</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Debugged Add book test case and Implemented Remove book test case</t>
+  </si>
+  <si>
+    <t>Unit Test Cases</t>
+  </si>
+  <si>
+    <t>Unit Test cases for Search Implemented</t>
+  </si>
+  <si>
+    <t>worked on some JUnit test cases for browse history</t>
+  </si>
+  <si>
+    <t>Coding and testing</t>
+  </si>
+  <si>
+    <t>Refactored presentation room code and worked on unit test cases for user login and registration.</t>
+  </si>
+  <si>
+    <t>Completed all the test cases</t>
+  </si>
+  <si>
+    <t>Test cases for AdminServices, updatenews and viewnews edit on cases printing</t>
+  </si>
+  <si>
+    <t>Test cases written</t>
+  </si>
+  <si>
     <t>Final review of the code and finishing off the object diagrams</t>
   </si>
   <si>
-    <t>User login and register add and remove user</t>
-  </si>
-  <si>
-    <t>Functionality implementation</t>
-  </si>
-  <si>
-    <t>Block and unBlock user update for admin</t>
-  </si>
-  <si>
-    <t>Functionality implementation for admin</t>
-  </si>
-  <si>
-    <t>Update without togglecase</t>
-  </si>
-  <si>
-    <t>Rework on functional case without togglecase</t>
-  </si>
-  <si>
-    <t>Test cases for User, blocking and userRepository</t>
-  </si>
-  <si>
-    <t>writing Junit testcases for the mentioned classes</t>
-  </si>
-  <si>
-    <t>Coding and debugging</t>
-  </si>
-  <si>
-    <t>Line edits, UI Changes, to string(), updateNews implementation</t>
-  </si>
-  <si>
-    <t>UI editing, implementation of toString() method and implementation of updateNews functionality</t>
-  </si>
-  <si>
-    <t>Implementing Admin services, view news toString()</t>
-  </si>
-  <si>
-    <t>Functionality implementation of adminServices and to string on viewNews</t>
-  </si>
-  <si>
-    <t>Debugging</t>
-  </si>
-  <si>
-    <t>UI changes and Junit 4 to 5 conversions and rewriting testcases</t>
-  </si>
-  <si>
-    <t>rewrk on testcases</t>
-  </si>
-  <si>
-    <t>Test cases for AdminServices, updatenews and viewnews edit on cases printing</t>
-  </si>
-  <si>
-    <t>Test cases written</t>
-  </si>
-  <si>
-    <t>Student Browse assets implemented along with advanced search</t>
-  </si>
-  <si>
-    <t>Browsing history Implemented</t>
-  </si>
-  <si>
-    <t>Code Refactoring and correcting the attributes in the classes</t>
-  </si>
-  <si>
-    <t>Review</t>
-  </si>
-  <si>
-    <t>Code Review</t>
-  </si>
-  <si>
-    <t>Reviewing peers code</t>
-  </si>
-  <si>
-    <t>Reviewing</t>
-  </si>
-  <si>
-    <t>Understanding the code classes with respect to class Diagram and reviewing peer's code for asset management and asset repository.</t>
-  </si>
-  <si>
-    <t>Developed an idea of which functionalities of assetmanagement and assetrepository class is to be used for implementing add and remove for book and other assets.</t>
-  </si>
-  <si>
-    <t>Coding for add and remove asset</t>
-  </si>
-  <si>
-    <t>Functionality developed for add and remove asset.</t>
-  </si>
-  <si>
-    <t>ReCoding for add and remove book as an individual asset rather then all asset in common because of different attributes.</t>
-  </si>
-  <si>
-    <t>Fully functional add and remove book code.</t>
-  </si>
-  <si>
-    <t>Refactoring and learning</t>
-  </si>
-  <si>
-    <t>Identified and reviewed mistakes as pointed out by peer. Learned new java concept of super and implmenting that in the add and remove book</t>
-  </si>
-  <si>
-    <t>Refactored Add and Remove Book code.</t>
-  </si>
-  <si>
-    <t>Update Book details coding</t>
-  </si>
-  <si>
-    <t>Developing Functionality and Debugging</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Test cases Review</t>
-  </si>
-  <si>
-    <t>Developing initial test case for adding a book</t>
-  </si>
-  <si>
-    <t>Raw version of code developed for adding a book</t>
-  </si>
-  <si>
-    <t>Developing test case for Remove book and debugging add book test case</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Debugged Add book test case and Implemented Remove book test case</t>
-  </si>
-  <si>
-    <t>Unit Test Cases</t>
-  </si>
-  <si>
-    <t>Unit Test cases for Search Implemented</t>
-  </si>
-  <si>
-    <t>worked on some JUnit test cases for browse history</t>
-  </si>
-  <si>
-    <t>Completed all the test cases</t>
+    <t>Presentation room code.</t>
+  </si>
+  <si>
+    <t>Refactored Presentation room code.</t>
   </si>
   <si>
     <t>Milestone 3</t>
@@ -1292,7 +1331,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1385,6 +1424,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="22" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="22" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1396,21 +1441,16 @@
     <xf numFmtId="15" fontId="1" fillId="2" borderId="4" xfId="22" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="22" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="22" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="22" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="22" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1767,29 +1807,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:S90"/>
+  <dimension ref="A3:S96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="D59" workbookViewId="0">
-      <selection activeCell="K64" sqref="K64"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.8888888888889" customWidth="1"/>
-    <col min="2" max="2" width="3.33333333333333" customWidth="1"/>
-    <col min="3" max="3" width="3.88888888888889" customWidth="1"/>
-    <col min="4" max="4" width="5.66666666666667" customWidth="1"/>
-    <col min="5" max="5" width="2.66666666666667" customWidth="1"/>
-    <col min="6" max="6" width="3.88888888888889" customWidth="1"/>
+    <col min="1" max="1" width="11.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="3.33636363636364" customWidth="1"/>
+    <col min="3" max="3" width="3.89090909090909" customWidth="1"/>
+    <col min="4" max="4" width="5.66363636363636" customWidth="1"/>
+    <col min="5" max="5" width="2.66363636363636" customWidth="1"/>
+    <col min="6" max="6" width="3.89090909090909" customWidth="1"/>
     <col min="7" max="7" width="3" customWidth="1"/>
-    <col min="8" max="8" width="15.4444444444444" customWidth="1"/>
-    <col min="9" max="9" width="15.3333333333333" customWidth="1"/>
-    <col min="10" max="10" width="21.8888888888889" customWidth="1"/>
-    <col min="11" max="11" width="25.4444444444444" customWidth="1"/>
-    <col min="19" max="19" width="35.6666666666667" customWidth="1"/>
+    <col min="8" max="8" width="15.4454545454545" customWidth="1"/>
+    <col min="9" max="9" width="15.3363636363636" customWidth="1"/>
+    <col min="10" max="10" width="21.8909090909091" customWidth="1"/>
+    <col min="11" max="11" width="25.4454545454545" customWidth="1"/>
+    <col min="19" max="19" width="35.6636363636364" customWidth="1"/>
     <col min="23" max="23" width="11" customWidth="1"/>
-    <col min="24" max="24" width="10.1111111111111" customWidth="1"/>
-    <col min="25" max="25" width="9.88888888888889" customWidth="1"/>
+    <col min="24" max="24" width="10.1090909090909" customWidth="1"/>
+    <col min="25" max="25" width="9.89090909090909" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" ht="16.5" customHeight="1" spans="8:19">
@@ -1799,18 +1839,18 @@
       <c r="I3" s="16"/>
       <c r="J3" s="17"/>
       <c r="K3" s="18"/>
-      <c r="S3" s="38" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" ht="15.9" spans="8:19">
+      <c r="S3" s="40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" ht="16" spans="8:19">
       <c r="H4" s="2"/>
       <c r="I4" s="19"/>
       <c r="J4" s="20"/>
       <c r="K4" s="21"/>
-      <c r="S4" s="38"/>
-    </row>
-    <row r="5" ht="29.55" spans="8:19">
+      <c r="S4" s="40"/>
+    </row>
+    <row r="5" ht="29.75" spans="8:19">
       <c r="H5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1821,7 +1861,7 @@
         <v>4</v>
       </c>
       <c r="K5" s="21"/>
-      <c r="S5" s="38"/>
+      <c r="S5" s="40"/>
     </row>
     <row r="6" spans="8:19">
       <c r="H6" s="4" t="s">
@@ -1834,7 +1874,7 @@
         <v>7</v>
       </c>
       <c r="K6" s="25"/>
-      <c r="S6" s="38"/>
+      <c r="S6" s="40"/>
     </row>
     <row r="7" spans="8:19">
       <c r="H7" s="4" t="s">
@@ -1847,7 +1887,7 @@
         <v>10</v>
       </c>
       <c r="K7" s="25"/>
-      <c r="S7" s="38"/>
+      <c r="S7" s="40"/>
     </row>
     <row r="8" spans="8:19">
       <c r="H8" s="4" t="s">
@@ -1860,7 +1900,7 @@
         <v>11</v>
       </c>
       <c r="K8" s="25"/>
-      <c r="S8" s="38"/>
+      <c r="S8" s="40"/>
     </row>
     <row r="9" spans="8:19">
       <c r="H9" s="4" t="s">
@@ -1873,7 +1913,7 @@
         <v>15</v>
       </c>
       <c r="K9" s="25"/>
-      <c r="S9" s="38"/>
+      <c r="S9" s="40"/>
     </row>
     <row r="10" spans="8:19">
       <c r="H10" s="4" t="s">
@@ -1886,7 +1926,7 @@
         <v>18</v>
       </c>
       <c r="K10" s="25"/>
-      <c r="S10" s="38"/>
+      <c r="S10" s="40"/>
     </row>
     <row r="11" spans="8:19">
       <c r="H11" s="5" t="s">
@@ -1899,7 +1939,7 @@
         <v>21</v>
       </c>
       <c r="K11" s="27"/>
-      <c r="S11" s="38"/>
+      <c r="S11" s="40"/>
     </row>
     <row r="12" spans="19:19">
       <c r="S12" t="s">
@@ -1942,8 +1982,8 @@
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
-      <c r="Q15" s="39"/>
-      <c r="R15" s="40"/>
+      <c r="Q15" s="41"/>
+      <c r="R15" s="42"/>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="6"/>
@@ -2371,7 +2411,7 @@
       </c>
       <c r="R24" s="36"/>
     </row>
-    <row r="25" ht="43.2" spans="1:18">
+    <row r="25" ht="43.5" spans="1:18">
       <c r="A25" s="13">
         <v>45326</v>
       </c>
@@ -2431,7 +2471,7 @@
       </c>
       <c r="R25" s="36"/>
     </row>
-    <row r="26" ht="86.4" spans="1:18">
+    <row r="26" ht="87" spans="1:18">
       <c r="A26" s="13">
         <v>45330</v>
       </c>
@@ -2527,7 +2567,7 @@
       </c>
       <c r="R27" s="36"/>
     </row>
-    <row r="28" ht="28.8" spans="1:18">
+    <row r="28" ht="29" spans="1:18">
       <c r="A28" s="13">
         <v>45333</v>
       </c>
@@ -2587,7 +2627,7 @@
       </c>
       <c r="R28" s="36"/>
     </row>
-    <row r="29" ht="57.6" spans="1:18">
+    <row r="29" ht="58" spans="1:18">
       <c r="A29" s="13">
         <v>45335</v>
       </c>
@@ -2647,7 +2687,7 @@
       </c>
       <c r="R29" s="36"/>
     </row>
-    <row r="30" ht="28.8" spans="1:18">
+    <row r="30" ht="29" spans="1:18">
       <c r="A30" s="13">
         <v>45338</v>
       </c>
@@ -2697,7 +2737,7 @@
       </c>
       <c r="R30" s="36"/>
     </row>
-    <row r="31" ht="43.2" spans="1:18">
+    <row r="31" ht="43.5" spans="1:18">
       <c r="A31" s="13">
         <v>45340</v>
       </c>
@@ -2747,7 +2787,7 @@
       </c>
       <c r="R31" s="36"/>
     </row>
-    <row r="32" ht="43.2" spans="1:18">
+    <row r="32" ht="43.5" spans="1:18">
       <c r="A32" s="13">
         <v>45340</v>
       </c>
@@ -2898,7 +2938,7 @@
         <v>63</v>
       </c>
       <c r="P35" s="36"/>
-      <c r="Q35" s="41"/>
+      <c r="Q35" s="43"/>
       <c r="R35" s="36">
         <f>SUM(L34:Q34)</f>
         <v>92.5</v>
@@ -2991,58 +3031,48 @@
         <v>69</v>
       </c>
       <c r="L38" s="37">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="L38:L78" si="10">B38*$I38</f>
         <v>0</v>
       </c>
       <c r="M38" s="9">
-        <f>C38*$I38</f>
+        <f t="shared" ref="M38:M78" si="11">C38*$I38</f>
         <v>0</v>
       </c>
       <c r="N38" s="9">
-        <f>D38*$I38</f>
+        <f t="shared" ref="N38:N78" si="12">D38*$I38</f>
         <v>0</v>
       </c>
       <c r="O38" s="9">
-        <f>E38*$I38</f>
+        <f t="shared" ref="O38:O78" si="13">E38*$I38</f>
         <v>0</v>
       </c>
       <c r="P38" s="9">
-        <f>F38*$I38</f>
+        <f t="shared" ref="P38:P78" si="14">F38*$I38</f>
         <v>0</v>
       </c>
       <c r="Q38" s="9">
-        <f>G38*$I38</f>
+        <f t="shared" ref="Q38:Q78" si="15">G38*$I38</f>
         <v>3.5</v>
       </c>
       <c r="R38" s="36"/>
     </row>
-    <row r="39" customFormat="1" ht="28.8" spans="1:18">
+    <row r="39" customFormat="1" ht="29" spans="1:18">
       <c r="A39" s="13">
-        <v>45347</v>
-      </c>
-      <c r="B39" s="14">
-        <v>1</v>
-      </c>
-      <c r="C39" s="14">
-        <v>1</v>
-      </c>
-      <c r="D39" s="14">
-        <v>1</v>
-      </c>
-      <c r="E39" s="14">
-        <v>1</v>
-      </c>
-      <c r="F39" s="14">
-        <v>1</v>
-      </c>
+        <v>45343</v>
+      </c>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
       <c r="G39" s="14">
         <v>1</v>
       </c>
       <c r="H39" s="14" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="I39" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J39" s="14" t="s">
         <v>70</v>
@@ -3051,202 +3081,182 @@
         <v>71</v>
       </c>
       <c r="L39" s="37">
-        <f t="shared" ref="L39:Q39" si="10">B39*$I39</f>
-        <v>3</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="M39" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N39" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O39" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P39" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="9">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="R39" s="36"/>
+    </row>
+    <row r="40" ht="29" spans="1:18">
+      <c r="A40" s="13">
+        <v>45344</v>
+      </c>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14">
+        <v>1</v>
+      </c>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="I40" s="33">
+        <v>3.5</v>
+      </c>
+      <c r="J40" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K40" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="L40" s="37">
         <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="N39" s="9">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="O39" s="9">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="P39" s="9">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="Q39" s="9">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="R39" s="36"/>
-    </row>
-    <row r="40" customFormat="1" spans="1:18">
-      <c r="A40" s="13">
-        <v>45349</v>
-      </c>
-      <c r="B40" s="14">
-        <v>1</v>
-      </c>
-      <c r="C40" s="14">
-        <v>1</v>
-      </c>
-      <c r="D40" s="14">
-        <v>1</v>
-      </c>
-      <c r="E40" s="14">
-        <v>1</v>
-      </c>
-      <c r="F40" s="14">
-        <v>1</v>
-      </c>
-      <c r="G40" s="14">
-        <v>1</v>
-      </c>
-      <c r="H40" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="I40" s="33">
-        <v>2</v>
-      </c>
-      <c r="J40" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="K40" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="L40" s="37">
-        <f t="shared" ref="L40:Q40" si="11">B40*$I40</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M40" s="9">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N40" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O40" s="9">
+        <f t="shared" si="13"/>
+        <v>3.5</v>
+      </c>
+      <c r="P40" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Q40" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="R40" s="36"/>
+    </row>
+    <row r="41" ht="43.5" spans="1:18">
+      <c r="A41" s="13">
+        <v>45344</v>
+      </c>
+      <c r="B41" s="14">
+        <v>1</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="I41" s="33">
+        <v>3.5</v>
+      </c>
+      <c r="J41" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K41" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="L41" s="37">
+        <f t="shared" si="10"/>
+        <v>3.5</v>
+      </c>
+      <c r="M41" s="9">
         <f t="shared" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="O40" s="9">
-        <f t="shared" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="P40" s="9">
-        <f t="shared" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="Q40" s="9">
-        <f t="shared" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="R40" s="36"/>
-    </row>
-    <row r="41" customFormat="1" ht="43.2" spans="1:18">
-      <c r="A41" s="13">
-        <v>45354</v>
-      </c>
-      <c r="B41" s="14">
-        <v>1</v>
-      </c>
-      <c r="C41" s="14">
-        <v>1</v>
-      </c>
-      <c r="D41" s="14">
-        <v>1</v>
-      </c>
-      <c r="E41" s="14">
-        <v>1</v>
-      </c>
-      <c r="F41" s="14">
-        <v>1</v>
-      </c>
-      <c r="G41" s="14">
-        <v>1</v>
-      </c>
-      <c r="H41" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="I41" s="33">
-        <v>3</v>
-      </c>
-      <c r="J41" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="K41" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="L41" s="37">
-        <f t="shared" ref="L41:Q41" si="12">B41*$I41</f>
-        <v>3</v>
-      </c>
-      <c r="M41" s="9">
-        <f t="shared" si="12"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N41" s="9">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O41" s="9">
-        <f t="shared" si="12"/>
-        <v>3</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="P41" s="9">
-        <f t="shared" si="12"/>
-        <v>3</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="Q41" s="9">
-        <f t="shared" si="12"/>
-        <v>3</v>
+        <f t="shared" si="15"/>
+        <v>0</v>
       </c>
       <c r="R41" s="36"/>
     </row>
-    <row r="42" ht="28.8" spans="1:18">
+    <row r="42" ht="29" spans="1:18">
       <c r="A42" s="13">
-        <v>45344</v>
-      </c>
-      <c r="B42" s="14"/>
+        <v>45345</v>
+      </c>
+      <c r="B42" s="14">
+        <v>1</v>
+      </c>
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
-      <c r="E42" s="14">
-        <v>1</v>
-      </c>
+      <c r="E42" s="14"/>
       <c r="F42" s="14"/>
       <c r="G42" s="14"/>
       <c r="H42" s="14" t="s">
         <v>65</v>
       </c>
       <c r="I42" s="33">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="J42" s="14" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K42" s="14" t="s">
         <v>75</v>
       </c>
       <c r="L42" s="37">
-        <f t="shared" ref="L42:L57" si="13">B42*$I42</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>3</v>
       </c>
       <c r="M42" s="9">
-        <f t="shared" ref="M42:M57" si="14">C42*$I42</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N42" s="9">
-        <f t="shared" ref="N42:N57" si="15">D42*$I42</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O42" s="9">
-        <f t="shared" ref="O42:O57" si="16">E42*$I42</f>
-        <v>3.5</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="P42" s="9">
-        <f t="shared" ref="P42:P57" si="17">F42*$I42</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q42" s="9">
-        <f t="shared" ref="Q42:Q47" si="18">G42*$I42</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R42" s="36"/>
     </row>
-    <row r="43" ht="28.8" spans="1:18">
+    <row r="43" ht="29" spans="1:18">
       <c r="A43" s="13">
         <v>45345</v>
       </c>
@@ -3271,32 +3281,32 @@
         <v>77</v>
       </c>
       <c r="L43" s="37">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N43" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O43" s="9">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="M43" s="9">
+        <v>3</v>
+      </c>
+      <c r="P43" s="9">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="N43" s="9">
+      <c r="Q43" s="9">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="O43" s="9">
-        <f t="shared" si="16"/>
-        <v>3</v>
-      </c>
-      <c r="P43" s="9">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="Q43" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
       <c r="R43" s="36"/>
     </row>
-    <row r="44" ht="28.8" spans="1:18">
+    <row r="44" ht="29" spans="1:18">
       <c r="A44" s="13">
         <v>45346</v>
       </c>
@@ -3321,242 +3331,252 @@
         <v>79</v>
       </c>
       <c r="L44" s="37">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M44" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N44" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O44" s="9">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="M44" s="9">
+        <v>1</v>
+      </c>
+      <c r="P44" s="9">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="N44" s="9">
+      <c r="Q44" s="9">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="O44" s="9">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-      <c r="P44" s="9">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="Q44" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
       <c r="R44" s="36"/>
     </row>
-    <row r="45" ht="43.2" spans="1:18">
+    <row r="45" ht="43.5" spans="1:18">
       <c r="A45" s="13">
-        <v>45350</v>
-      </c>
-      <c r="B45" s="14"/>
+        <v>45346</v>
+      </c>
+      <c r="B45" s="14">
+        <v>1</v>
+      </c>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
-      <c r="E45" s="14">
-        <v>1</v>
-      </c>
+      <c r="E45" s="14"/>
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
       <c r="H45" s="14" t="s">
         <v>65</v>
       </c>
       <c r="I45" s="33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J45" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K45" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="K45" s="14" t="s">
-        <v>81</v>
-      </c>
       <c r="L45" s="37">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="M45" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N45" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O45" s="9">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="M45" s="9">
+      <c r="P45" s="9">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="N45" s="9">
+      <c r="Q45" s="9">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="O45" s="9">
-        <f t="shared" si="16"/>
-        <v>4</v>
-      </c>
-      <c r="P45" s="9">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="Q45" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
       <c r="R45" s="36"/>
     </row>
-    <row r="46" ht="57.6" spans="1:18">
+    <row r="46" ht="101.5" spans="1:18">
       <c r="A46" s="13">
-        <v>45351</v>
+        <v>45346</v>
       </c>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
       <c r="D46" s="14"/>
-      <c r="E46" s="14">
-        <v>1</v>
-      </c>
-      <c r="F46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14">
+        <v>1</v>
+      </c>
       <c r="G46" s="14"/>
       <c r="H46" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="I46" s="33">
+        <v>3.5</v>
+      </c>
+      <c r="J46" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="I46" s="33">
-        <v>6</v>
-      </c>
-      <c r="J46" s="14" t="s">
+      <c r="K46" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="K46" s="14" t="s">
+      <c r="L46" s="37">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M46" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N46" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O46" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P46" s="9">
+        <f t="shared" si="14"/>
+        <v>3.5</v>
+      </c>
+      <c r="Q46" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="R46" s="36"/>
+    </row>
+    <row r="47" customFormat="1" ht="29" spans="1:18">
+      <c r="A47" s="13">
+        <v>45347</v>
+      </c>
+      <c r="B47" s="14">
+        <v>1</v>
+      </c>
+      <c r="C47" s="14">
+        <v>1</v>
+      </c>
+      <c r="D47" s="14">
+        <v>1</v>
+      </c>
+      <c r="E47" s="14">
+        <v>1</v>
+      </c>
+      <c r="F47" s="14">
+        <v>1</v>
+      </c>
+      <c r="G47" s="14">
+        <v>1</v>
+      </c>
+      <c r="H47" s="14" t="s">
         <v>84</v>
-      </c>
-      <c r="L46" s="37">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="M46" s="9">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="N46" s="9">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="O46" s="9">
-        <f t="shared" si="16"/>
-        <v>6</v>
-      </c>
-      <c r="P46" s="9">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="Q46" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="R46" s="36"/>
-    </row>
-    <row r="47" ht="43.2" spans="1:18">
-      <c r="A47" s="13">
-        <v>45352</v>
-      </c>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14">
-        <v>1</v>
-      </c>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14" t="s">
-        <v>65</v>
       </c>
       <c r="I47" s="33">
         <v>3</v>
       </c>
       <c r="J47" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="K47" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="K47" s="14" t="s">
-        <v>86</v>
-      </c>
       <c r="L47" s="37">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="M47" s="9">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="N47" s="9">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="O47" s="9">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="M47" s="9">
+        <v>3</v>
+      </c>
+      <c r="P47" s="9">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="N47" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q47" s="9">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="O47" s="9">
-        <f t="shared" si="16"/>
         <v>3</v>
       </c>
-      <c r="P47" s="9">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="Q47" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
       <c r="R47" s="36"/>
     </row>
-    <row r="48" ht="43.2" spans="1:18">
+    <row r="48" customFormat="1" ht="29" spans="1:18">
       <c r="A48" s="13">
-        <v>45353</v>
+        <v>45347</v>
       </c>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
       <c r="D48" s="14"/>
-      <c r="E48" s="14">
-        <v>1</v>
-      </c>
+      <c r="E48" s="14"/>
       <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
+      <c r="G48" s="14">
+        <v>1</v>
+      </c>
       <c r="H48" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="I48" s="33">
+        <v>1</v>
+      </c>
+      <c r="J48" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="K48" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="I48" s="33">
-        <v>2</v>
-      </c>
-      <c r="J48" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="K48" s="14" t="s">
-        <v>89</v>
-      </c>
       <c r="L48" s="37">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M48" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N48" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O48" s="9">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="M48" s="9">
+      <c r="P48" s="9">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="N48" s="9">
+      <c r="Q48" s="9">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="O48" s="9">
-        <f t="shared" si="16"/>
-        <v>2</v>
-      </c>
-      <c r="P48" s="9">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="Q48" s="9">
-        <f t="shared" ref="Q48:Q53" si="19">G48*$I48</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R48" s="36"/>
     </row>
-    <row r="49" ht="72" spans="1:18">
+    <row r="49" ht="29" spans="1:18">
       <c r="A49" s="13">
-        <v>45354</v>
+        <v>45347</v>
       </c>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
-      <c r="E49" s="14">
-        <v>1</v>
-      </c>
-      <c r="F49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14">
+        <v>1</v>
+      </c>
       <c r="G49" s="14"/>
       <c r="H49" s="14" t="s">
         <v>65</v>
@@ -3565,40 +3585,40 @@
         <v>4</v>
       </c>
       <c r="J49" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K49" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L49" s="37">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M49" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N49" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O49" s="9">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="M49" s="9">
+      <c r="P49" s="9">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="N49" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q49" s="9">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="O49" s="9">
-        <f t="shared" si="16"/>
-        <v>4</v>
-      </c>
-      <c r="P49" s="9">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="Q49" s="9">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
       <c r="R49" s="36"/>
     </row>
-    <row r="50" ht="43.2" spans="1:18">
+    <row r="50" spans="1:18">
       <c r="A50" s="13">
-        <v>45344</v>
+        <v>45347</v>
       </c>
       <c r="B50" s="14">
         <v>1</v>
@@ -3609,54 +3629,54 @@
       <c r="F50" s="14"/>
       <c r="G50" s="14"/>
       <c r="H50" s="14" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="I50" s="33">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="J50" s="14" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="K50" s="14" t="s">
         <v>92</v>
       </c>
       <c r="L50" s="37">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="M50" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N50" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O50" s="9">
         <f t="shared" si="13"/>
-        <v>3.5</v>
-      </c>
-      <c r="M50" s="9">
+        <v>0</v>
+      </c>
+      <c r="P50" s="9">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="N50" s="9">
+      <c r="Q50" s="9">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="O50" s="9">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="P50" s="9">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="Q50" s="9">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
       <c r="R50" s="36"/>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" ht="87" spans="1:18">
       <c r="A51" s="13">
-        <v>45345</v>
-      </c>
-      <c r="B51" s="14">
-        <v>1</v>
-      </c>
+        <v>45347</v>
+      </c>
+      <c r="B51" s="14"/>
       <c r="C51" s="14"/>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
+      <c r="F51" s="14">
+        <v>1</v>
+      </c>
       <c r="G51" s="14"/>
       <c r="H51" s="14" t="s">
         <v>65</v>
@@ -3665,239 +3685,250 @@
         <v>3</v>
       </c>
       <c r="J51" s="14" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="K51" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L51" s="37">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M51" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N51" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O51" s="9">
         <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P51" s="9">
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
-      <c r="M51" s="9">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="N51" s="9">
+      <c r="Q51" s="9">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="O51" s="9">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="P51" s="9">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="Q51" s="9">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
       <c r="R51" s="36"/>
     </row>
-    <row r="52" ht="43.2" spans="1:18">
+    <row r="52" ht="101.5" spans="1:18">
       <c r="A52" s="13">
-        <v>45346</v>
-      </c>
-      <c r="B52" s="14">
-        <v>1</v>
-      </c>
+        <v>45348</v>
+      </c>
+      <c r="B52" s="14"/>
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
+      <c r="F52" s="14">
+        <v>1</v>
+      </c>
       <c r="G52" s="14"/>
       <c r="H52" s="14" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="I52" s="33">
+        <v>4</v>
+      </c>
+      <c r="J52" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="K52" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="L52" s="37">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M52" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N52" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O52" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P52" s="9">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="Q52" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="R52" s="36"/>
+    </row>
+    <row r="53" customFormat="1" spans="1:18">
+      <c r="A53" s="13">
+        <v>45349</v>
+      </c>
+      <c r="B53" s="14">
+        <v>1</v>
+      </c>
+      <c r="C53" s="14">
+        <v>1</v>
+      </c>
+      <c r="D53" s="14">
+        <v>1</v>
+      </c>
+      <c r="E53" s="14">
+        <v>1</v>
+      </c>
+      <c r="F53" s="14">
+        <v>1</v>
+      </c>
+      <c r="G53" s="14">
+        <v>1</v>
+      </c>
+      <c r="H53" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="I53" s="33">
         <v>2</v>
       </c>
-      <c r="J52" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="K52" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="L52" s="37">
+      <c r="J53" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="K53" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="L53" s="37">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="M53" s="9">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="N53" s="9">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="O53" s="9">
         <f t="shared" si="13"/>
         <v>2</v>
       </c>
-      <c r="M52" s="9">
+      <c r="P53" s="9">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="N52" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q53" s="9">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="O52" s="9">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="P52" s="9">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="Q52" s="9">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="R52" s="36"/>
-    </row>
-    <row r="53" spans="1:18">
-      <c r="A53" s="13">
-        <v>45347</v>
-      </c>
-      <c r="B53" s="14">
-        <v>1</v>
-      </c>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="I53" s="33">
         <v>2</v>
       </c>
-      <c r="J53" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="K53" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="L53" s="37">
-        <f t="shared" si="13"/>
-        <v>2</v>
-      </c>
-      <c r="M53" s="9">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="N53" s="9">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="O53" s="9">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="P53" s="9">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="Q53" s="9">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
       <c r="R53" s="36"/>
     </row>
-    <row r="54" spans="1:17">
+    <row r="54" customFormat="1" ht="29" spans="1:18">
       <c r="A54" s="13">
-        <v>45350</v>
-      </c>
-      <c r="B54" s="14">
-        <v>1</v>
-      </c>
+        <v>45349</v>
+      </c>
+      <c r="B54" s="14"/>
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
       <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
+      <c r="G54" s="14">
+        <v>1</v>
+      </c>
       <c r="H54" s="14" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="I54" s="33">
-        <v>1</v>
-      </c>
-      <c r="J54" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="K54" s="14" t="s">
-        <v>97</v>
+        <v>3</v>
+      </c>
+      <c r="J54" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="K54" s="39" t="s">
+        <v>100</v>
       </c>
       <c r="L54" s="37">
-        <f>B54*$I54</f>
-        <v>1</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="M54" s="9">
-        <f>C54*$I54</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N54" s="9">
-        <f>D54*$I54</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O54" s="9">
-        <f>E54*$I54</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P54" s="9">
-        <f>F54*$I54</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q54" s="9">
-        <f>G54*$I54</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" customFormat="1" spans="1:18">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="R54" s="36"/>
+    </row>
+    <row r="55" ht="43.5" spans="1:18">
       <c r="A55" s="13">
-        <v>45351</v>
-      </c>
-      <c r="B55" s="14">
-        <v>1</v>
-      </c>
+        <v>45350</v>
+      </c>
+      <c r="B55" s="14"/>
       <c r="C55" s="14"/>
       <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
+      <c r="E55" s="14">
+        <v>1</v>
+      </c>
       <c r="F55" s="14"/>
       <c r="G55" s="14"/>
       <c r="H55" s="14" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="I55" s="33">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J55" s="14" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="K55" s="14" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="L55" s="37">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M55" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N55" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O55" s="9">
         <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="M55" s="9">
+        <v>4</v>
+      </c>
+      <c r="P55" s="9">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="N55" s="9">
+      <c r="Q55" s="9">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="O55" s="9">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="P55" s="9">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="Q55" s="9">
-        <f>G55*$I55</f>
-        <v>0</v>
-      </c>
       <c r="R55" s="36"/>
     </row>
-    <row r="56" spans="1:18">
+    <row r="56" spans="1:17">
       <c r="A56" s="13">
-        <v>45352</v>
+        <v>45350</v>
       </c>
       <c r="B56" s="14">
         <v>1</v>
@@ -3908,217 +3939,243 @@
       <c r="F56" s="14"/>
       <c r="G56" s="14"/>
       <c r="H56" s="14" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I56" s="33">
         <v>1</v>
       </c>
       <c r="J56" s="14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="K56" s="14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="L56" s="37">
-        <f>B56*$I56</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="M56" s="9">
-        <f>C56*$I56</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N56" s="9">
-        <f>D56*$I56</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O56" s="9">
-        <f>E56*$I56</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P56" s="9">
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q56" s="9">
-        <f>G56*$I56</f>
-        <v>0</v>
-      </c>
-      <c r="R56" s="36"/>
-    </row>
-    <row r="57" ht="100.8" spans="1:18">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" ht="58" spans="1:18">
       <c r="A57" s="13">
-        <v>45346</v>
+        <v>45351</v>
       </c>
       <c r="B57" s="14"/>
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14">
-        <v>1</v>
-      </c>
+      <c r="E57" s="14">
+        <v>1</v>
+      </c>
+      <c r="F57" s="14"/>
       <c r="G57" s="14"/>
       <c r="H57" s="14" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="I57" s="33">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="J57" s="14" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="K57" s="14" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="L57" s="37">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M57" s="9">
-        <v>0</v>
-      </c>
-      <c r="N57" s="9"/>
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N57" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
       <c r="O57" s="9">
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>6</v>
       </c>
       <c r="P57" s="9">
-        <v>3.5</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="Q57" s="9">
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R57" s="36"/>
     </row>
-    <row r="58" ht="28.8" spans="1:18">
+    <row r="58" customFormat="1" spans="1:18">
       <c r="A58" s="13">
-        <v>45347</v>
-      </c>
-      <c r="B58" s="14"/>
+        <v>45351</v>
+      </c>
+      <c r="B58" s="14">
+        <v>1</v>
+      </c>
       <c r="C58" s="14"/>
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
-      <c r="F58" s="14">
-        <v>1</v>
-      </c>
+      <c r="F58" s="14"/>
       <c r="G58" s="14"/>
       <c r="H58" s="14" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="I58" s="33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J58" s="14" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="K58" s="14" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L58" s="37">
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>1</v>
       </c>
       <c r="M58" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N58" s="9">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O58" s="9">
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P58" s="9">
-        <v>4</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="Q58" s="9">
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R58" s="36"/>
     </row>
-    <row r="59" ht="86.4" spans="1:18">
+    <row r="59" customFormat="1" ht="29" spans="1:18">
       <c r="A59" s="13">
-        <v>45347</v>
+        <v>45351</v>
       </c>
       <c r="B59" s="14"/>
       <c r="C59" s="14"/>
       <c r="D59" s="14"/>
       <c r="E59" s="14"/>
-      <c r="F59" s="14">
-        <v>1</v>
-      </c>
-      <c r="G59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14">
+        <v>1</v>
+      </c>
       <c r="H59" s="14" t="s">
         <v>65</v>
       </c>
       <c r="I59" s="33">
-        <v>3</v>
-      </c>
-      <c r="J59" s="14" t="s">
-        <v>103</v>
+        <v>3.5</v>
+      </c>
+      <c r="J59" s="38" t="s">
+        <v>99</v>
       </c>
       <c r="K59" s="14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L59" s="37">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M59" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N59" s="9">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O59" s="9">
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P59" s="9">
-        <v>3</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="Q59" s="9">
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>3.5</v>
       </c>
       <c r="R59" s="36"/>
     </row>
-    <row r="60" ht="86.4" spans="1:18">
+    <row r="60" spans="1:18">
       <c r="A60" s="13">
-        <v>45348</v>
-      </c>
-      <c r="B60" s="14"/>
+        <v>45352</v>
+      </c>
+      <c r="B60" s="14">
+        <v>1</v>
+      </c>
       <c r="C60" s="14"/>
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
-      <c r="F60" s="14">
-        <v>1</v>
-      </c>
+      <c r="F60" s="14"/>
       <c r="G60" s="14"/>
       <c r="H60" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="I60" s="33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J60" s="14" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="K60" s="14" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="L60" s="37">
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>1</v>
       </c>
       <c r="M60" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N60" s="9">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O60" s="9">
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P60" s="9">
-        <v>4</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="Q60" s="9">
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R60" s="36"/>
     </row>
-    <row r="61" ht="28.8" spans="1:18">
+    <row r="61" ht="29" spans="1:18">
       <c r="A61" s="13">
         <v>45352</v>
       </c>
@@ -4137,27 +4194,33 @@
         <v>2</v>
       </c>
       <c r="J61" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="K61" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="K61" s="14" t="s">
-        <v>109</v>
-      </c>
       <c r="L61" s="37">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M61" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N61" s="9">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O61" s="9">
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P61" s="9">
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="Q61" s="9">
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R61" s="36"/>
@@ -4175,84 +4238,96 @@
       </c>
       <c r="G62" s="14"/>
       <c r="H62" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I62" s="33">
         <v>4</v>
       </c>
       <c r="J62" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K62" s="14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="L62" s="37">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M62" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N62" s="9">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O62" s="9">
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P62" s="9">
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>4</v>
       </c>
       <c r="Q62" s="9">
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R62" s="36"/>
     </row>
-    <row r="63" ht="28.8" spans="1:18">
+    <row r="63" ht="43.5" spans="1:18">
       <c r="A63" s="13">
         <v>45352</v>
       </c>
       <c r="B63" s="14"/>
       <c r="C63" s="14"/>
       <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14">
-        <v>1</v>
-      </c>
+      <c r="E63" s="14">
+        <v>1</v>
+      </c>
+      <c r="F63" s="14"/>
       <c r="G63" s="14"/>
       <c r="H63" s="14" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="I63" s="33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J63" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="K63" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="K63" s="14" t="s">
-        <v>113</v>
-      </c>
       <c r="L63" s="37">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M63" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N63" s="9">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O63" s="9">
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>3</v>
       </c>
       <c r="P63" s="9">
-        <v>4</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="Q63" s="9">
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R63" s="36"/>
     </row>
-    <row r="64" ht="57.6" spans="1:18">
+    <row r="64" ht="29" spans="1:18">
       <c r="A64" s="13">
-        <v>45353</v>
+        <v>45352</v>
       </c>
       <c r="B64" s="14"/>
       <c r="C64" s="14"/>
@@ -4263,54 +4338,60 @@
       </c>
       <c r="G64" s="14"/>
       <c r="H64" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I64" s="33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J64" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="K64" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="K64" s="14" t="s">
-        <v>115</v>
-      </c>
       <c r="L64" s="37">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M64" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N64" s="9">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O64" s="9">
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P64" s="9">
-        <v>4</v>
+        <f t="shared" si="14"/>
+        <v>2</v>
       </c>
       <c r="Q64" s="9">
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R64" s="36"/>
     </row>
-    <row r="65" ht="28.8" spans="1:18">
+    <row r="65" ht="43.5" spans="1:18">
       <c r="A65" s="13">
         <v>45353</v>
       </c>
-      <c r="B65" s="14">
-        <v>1</v>
-      </c>
+      <c r="B65" s="14"/>
       <c r="C65" s="14"/>
       <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
+      <c r="E65" s="14">
+        <v>1</v>
+      </c>
       <c r="F65" s="14"/>
       <c r="G65" s="14"/>
       <c r="H65" s="14" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="I65" s="33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J65" s="14" t="s">
         <v>116</v>
@@ -4319,294 +4400,490 @@
         <v>117</v>
       </c>
       <c r="L65" s="37">
-        <f>B65*$I65</f>
-        <v>4</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="M65" s="9">
-        <f>C65*$I65</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N65" s="9">
-        <f>D65*$I65</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O65" s="9">
-        <f>E65*$I65</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>2</v>
       </c>
       <c r="P65" s="9">
-        <f>F65*$I65</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q65" s="9">
-        <f>G65*$I65</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R65" s="36"/>
     </row>
-    <row r="66" ht="28.8" spans="1:18">
+    <row r="66" ht="43.5" spans="1:18">
       <c r="A66" s="13">
-        <v>45354</v>
-      </c>
-      <c r="B66" s="14">
-        <v>1</v>
-      </c>
+        <v>45353</v>
+      </c>
+      <c r="B66" s="14"/>
       <c r="C66" s="14"/>
       <c r="D66" s="14"/>
       <c r="E66" s="14"/>
       <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
+      <c r="G66" s="14">
+        <v>1</v>
+      </c>
       <c r="H66" s="14" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="I66" s="33">
-        <v>4</v>
-      </c>
-      <c r="J66" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="K66" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J66" s="38" t="s">
         <v>118</v>
       </c>
+      <c r="K66" s="39" t="s">
+        <v>119</v>
+      </c>
       <c r="L66" s="37">
-        <f>B66*$I66</f>
-        <v>4</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="M66" s="9">
-        <f>C66*$I66</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N66" s="9">
-        <f>D66*$I66</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O66" s="9">
-        <f>E66*$I66</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P66" s="9">
-        <f>F66*$I66</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q66" s="9">
-        <f>G66*$I66</f>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>3</v>
       </c>
       <c r="R66" s="36"/>
     </row>
-    <row r="67" customFormat="1" spans="1:18">
+    <row r="67" ht="58" spans="1:18">
       <c r="A67" s="13">
-        <v>45354</v>
-      </c>
-      <c r="B67" s="14">
-        <v>1</v>
-      </c>
+        <v>45353</v>
+      </c>
+      <c r="B67" s="14"/>
       <c r="C67" s="14"/>
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
+      <c r="F67" s="14">
+        <v>1</v>
+      </c>
       <c r="G67" s="14"/>
       <c r="H67" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I67" s="33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J67" s="14" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="K67" s="14" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="L67" s="37">
-        <f>B67*$I67</f>
-        <v>3</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="M67" s="9">
-        <f>C67*$I67</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N67" s="9">
-        <f>D67*$I67</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O67" s="9">
-        <f>E67*$I67</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P67" s="9">
-        <f>F67*$I67</f>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>4</v>
       </c>
       <c r="Q67" s="9">
-        <f>G67*$I67</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R67" s="36"/>
     </row>
-    <row r="68" spans="1:18">
-      <c r="A68" s="13"/>
-      <c r="B68" s="14"/>
+    <row r="68" ht="29" spans="1:18">
+      <c r="A68" s="13">
+        <v>45353</v>
+      </c>
+      <c r="B68" s="14">
+        <v>1</v>
+      </c>
       <c r="C68" s="14"/>
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
       <c r="F68" s="14"/>
       <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="33"/>
-      <c r="J68" s="14"/>
-      <c r="K68" s="14"/>
+      <c r="H68" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I68" s="33">
+        <v>4</v>
+      </c>
+      <c r="J68" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="K68" s="14" t="s">
+        <v>123</v>
+      </c>
       <c r="L68" s="37">
-        <f>B68*$I68</f>
-        <v>0</v>
-      </c>
-      <c r="M68" s="46">
-        <f>C68*$I68</f>
-        <v>0</v>
-      </c>
-      <c r="N68" s="46">
-        <f>D68*$I68</f>
-        <v>0</v>
-      </c>
-      <c r="O68" s="46">
-        <f>E68*$I68</f>
-        <v>0</v>
-      </c>
-      <c r="P68" s="47">
-        <f>F68*$I68</f>
-        <v>0</v>
-      </c>
-      <c r="Q68" s="47">
-        <f>G68*$I68</f>
-        <v>0</v>
-      </c>
-      <c r="R68" s="36">
-        <f>SUM(L75:Q75)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18">
-      <c r="A69" s="15"/>
-      <c r="H69" s="35"/>
-      <c r="K69" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="L69" s="36">
-        <f t="shared" ref="L69:Q69" si="20">SUM(L37:L68)</f>
-        <v>32.5</v>
-      </c>
-      <c r="M69" s="36">
-        <f t="shared" si="20"/>
-        <v>8</v>
-      </c>
-      <c r="N69" s="36">
-        <f t="shared" si="20"/>
-        <v>8</v>
-      </c>
-      <c r="O69" s="36">
-        <f t="shared" si="20"/>
-        <v>34.5</v>
-      </c>
-      <c r="P69" s="36">
-        <f t="shared" si="20"/>
-        <v>32.5</v>
-      </c>
-      <c r="Q69" s="36">
-        <f t="shared" si="20"/>
-        <v>14</v>
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="M68" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N68" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O68" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P68" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Q68" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="R68" s="36"/>
+    </row>
+    <row r="69" ht="29" spans="1:18">
+      <c r="A69" s="13">
+        <v>45354</v>
+      </c>
+      <c r="B69" s="14">
+        <v>1</v>
+      </c>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I69" s="33">
+        <v>4</v>
+      </c>
+      <c r="J69" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="K69" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="L69" s="37">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="M69" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N69" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O69" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P69" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Q69" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
       </c>
       <c r="R69" s="36"/>
     </row>
-    <row r="70" spans="1:18">
-      <c r="A70" s="15"/>
-      <c r="K70" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="P70" s="36"/>
-      <c r="Q70" s="36"/>
-      <c r="R70" s="36">
-        <f>SUM(L69:Q69)</f>
-        <v>129.5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18">
-      <c r="A71" s="15"/>
-      <c r="P71" s="36"/>
-      <c r="Q71" s="41"/>
+    <row r="70" customFormat="1" ht="58" spans="1:18">
+      <c r="A70" s="13">
+        <v>45354</v>
+      </c>
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14">
+        <v>1</v>
+      </c>
+      <c r="H70" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="I70" s="33">
+        <v>4.5</v>
+      </c>
+      <c r="J70" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="K70" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="L70" s="37">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M70" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N70" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O70" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P70" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Q70" s="9">
+        <f t="shared" si="15"/>
+        <v>4.5</v>
+      </c>
+      <c r="R70" s="36"/>
+    </row>
+    <row r="71" customFormat="1" spans="1:18">
+      <c r="A71" s="13">
+        <v>45354</v>
+      </c>
+      <c r="B71" s="14">
+        <v>1</v>
+      </c>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I71" s="33">
+        <v>3</v>
+      </c>
+      <c r="J71" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="K71" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="L71" s="37">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="M71" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N71" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O71" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P71" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Q71" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
       <c r="R71" s="36"/>
     </row>
-    <row r="72" spans="1:18">
-      <c r="A72" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="L72" s="31"/>
-      <c r="M72" s="11"/>
-      <c r="N72" s="11"/>
-      <c r="O72" s="11"/>
-      <c r="P72" s="32"/>
-      <c r="Q72" s="34"/>
+    <row r="72" ht="72.5" spans="1:18">
+      <c r="A72" s="13">
+        <v>45354</v>
+      </c>
+      <c r="B72" s="14"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14">
+        <v>1</v>
+      </c>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="I72" s="33">
+        <v>4</v>
+      </c>
+      <c r="J72" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="K72" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="L72" s="37">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M72" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N72" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O72" s="9">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="P72" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Q72" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
       <c r="R72" s="36"/>
     </row>
-    <row r="73" spans="1:18">
-      <c r="A73" s="42"/>
-      <c r="B73" s="43"/>
-      <c r="C73" s="43"/>
-      <c r="D73" s="43"/>
-      <c r="E73" s="43"/>
-      <c r="F73" s="43"/>
-      <c r="G73" s="43"/>
-      <c r="H73" s="43"/>
-      <c r="I73" s="48"/>
-      <c r="J73" s="43"/>
-      <c r="K73" s="49"/>
+    <row r="73" customFormat="1" ht="43.5" spans="1:18">
+      <c r="A73" s="13">
+        <v>45354</v>
+      </c>
+      <c r="B73" s="14">
+        <v>1</v>
+      </c>
+      <c r="C73" s="14">
+        <v>1</v>
+      </c>
+      <c r="D73" s="14">
+        <v>1</v>
+      </c>
+      <c r="E73" s="14">
+        <v>1</v>
+      </c>
+      <c r="F73" s="14">
+        <v>1</v>
+      </c>
+      <c r="G73" s="14">
+        <v>1</v>
+      </c>
+      <c r="H73" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="I73" s="33">
+        <v>3</v>
+      </c>
+      <c r="J73" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="K73" s="14" t="s">
+        <v>130</v>
+      </c>
       <c r="L73" s="37">
-        <f t="shared" ref="L73" si="21">B73*$I73</f>
-        <v>0</v>
-      </c>
-      <c r="M73" s="46">
-        <f t="shared" ref="M73" si="22">C73*$I73</f>
-        <v>0</v>
-      </c>
-      <c r="N73" s="46">
-        <f t="shared" ref="N73" si="23">D73*$I73</f>
-        <v>0</v>
-      </c>
-      <c r="O73" s="46">
-        <f t="shared" ref="O73" si="24">E73*$I73</f>
-        <v>0</v>
-      </c>
-      <c r="P73" s="47">
-        <f t="shared" ref="P73:Q73" si="25">F73*$I73</f>
-        <v>0</v>
-      </c>
-      <c r="Q73" s="47">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="M73" s="9">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="N73" s="9">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="O73" s="9">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="P73" s="9">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="Q73" s="9">
+        <f t="shared" si="15"/>
+        <v>3</v>
       </c>
       <c r="R73" s="36"/>
     </row>
-    <row r="74" spans="1:18">
-      <c r="A74" s="42"/>
-      <c r="B74" s="43"/>
-      <c r="C74" s="43"/>
-      <c r="D74" s="43"/>
-      <c r="E74" s="43"/>
-      <c r="F74" s="43"/>
-      <c r="G74" s="43"/>
-      <c r="H74" s="43"/>
-      <c r="I74" s="48"/>
-      <c r="J74" s="43"/>
-      <c r="K74" s="49"/>
-      <c r="L74" s="35"/>
-      <c r="M74" s="35"/>
-      <c r="N74" s="35"/>
-      <c r="O74" s="35"/>
-      <c r="P74" s="34"/>
-      <c r="Q74" s="34"/>
-      <c r="R74" s="36">
-        <f>SUM(L81:P81)</f>
-        <v>0</v>
-      </c>
+    <row r="74" ht="29" spans="1:18">
+      <c r="A74" s="13">
+        <v>45355</v>
+      </c>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14">
+        <v>1</v>
+      </c>
+      <c r="H74" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="I74" s="33">
+        <v>2</v>
+      </c>
+      <c r="J74" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="K74" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="L74" s="37">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M74" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N74" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O74" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P74" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Q74" s="9">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="R74" s="36"/>
     </row>
     <row r="75" spans="1:18">
       <c r="A75" s="15"/>
@@ -4614,29 +4891,29 @@
       <c r="K75" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="L75">
-        <f>SUM(L73:L74)</f>
-        <v>0</v>
-      </c>
-      <c r="M75">
-        <f t="shared" ref="M75" si="26">SUM(M73:M74)</f>
-        <v>0</v>
-      </c>
-      <c r="N75">
-        <f t="shared" ref="N75" si="27">SUM(N73:N74)</f>
-        <v>0</v>
-      </c>
-      <c r="O75">
-        <f t="shared" ref="O75" si="28">SUM(O73:O74)</f>
-        <v>0</v>
-      </c>
-      <c r="P75" s="36">
-        <f t="shared" ref="P75:Q75" si="29">SUM(P73:P74)</f>
-        <v>0</v>
-      </c>
-      <c r="Q75" s="36">
-        <f t="shared" si="29"/>
-        <v>0</v>
+      <c r="L75" s="47">
+        <f t="shared" ref="L75:Q75" si="16">SUM(L37:L74)</f>
+        <v>32.5</v>
+      </c>
+      <c r="M75" s="47">
+        <f t="shared" si="16"/>
+        <v>8</v>
+      </c>
+      <c r="N75" s="47">
+        <f t="shared" si="16"/>
+        <v>8</v>
+      </c>
+      <c r="O75" s="47">
+        <f t="shared" si="16"/>
+        <v>34.5</v>
+      </c>
+      <c r="P75" s="47">
+        <f t="shared" si="16"/>
+        <v>34.5</v>
+      </c>
+      <c r="Q75" s="47">
+        <f t="shared" si="16"/>
+        <v>33</v>
       </c>
       <c r="R75" s="36"/>
     </row>
@@ -4647,18 +4924,20 @@
       </c>
       <c r="P76" s="36"/>
       <c r="Q76" s="36"/>
-      <c r="R76" s="36"/>
+      <c r="R76" s="36">
+        <f>SUM(L75:Q75)</f>
+        <v>150.5</v>
+      </c>
     </row>
     <row r="77" spans="1:18">
       <c r="A77" s="15"/>
-      <c r="K77" s="35"/>
       <c r="P77" s="36"/>
-      <c r="Q77" s="41"/>
+      <c r="Q77" s="43"/>
       <c r="R77" s="36"/>
     </row>
     <row r="78" spans="1:18">
       <c r="A78" s="15" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="L78" s="31"/>
       <c r="M78" s="11"/>
@@ -4669,65 +4948,65 @@
       <c r="R78" s="36"/>
     </row>
     <row r="79" spans="1:18">
-      <c r="A79" s="42"/>
-      <c r="B79" s="43"/>
-      <c r="C79" s="43"/>
-      <c r="D79" s="43"/>
-      <c r="E79" s="43"/>
-      <c r="F79" s="43"/>
-      <c r="G79" s="43"/>
-      <c r="H79" s="43"/>
+      <c r="A79" s="44"/>
+      <c r="B79" s="38"/>
+      <c r="C79" s="38"/>
+      <c r="D79" s="38"/>
+      <c r="E79" s="38"/>
+      <c r="F79" s="38"/>
+      <c r="G79" s="38"/>
+      <c r="H79" s="38"/>
       <c r="I79" s="48"/>
-      <c r="J79" s="43"/>
-      <c r="K79" s="49"/>
+      <c r="J79" s="38"/>
+      <c r="K79" s="39"/>
       <c r="L79" s="37">
-        <f t="shared" ref="L79" si="30">B79*$I79</f>
-        <v>0</v>
-      </c>
-      <c r="M79" s="46">
-        <f t="shared" ref="M79" si="31">C79*$I79</f>
-        <v>0</v>
-      </c>
-      <c r="N79" s="46">
-        <f t="shared" ref="N79" si="32">D79*$I79</f>
-        <v>0</v>
-      </c>
-      <c r="O79" s="46">
-        <f t="shared" ref="O79" si="33">E79*$I79</f>
-        <v>0</v>
-      </c>
-      <c r="P79" s="47">
-        <f t="shared" ref="P79:Q79" si="34">F79*$I79</f>
-        <v>0</v>
-      </c>
-      <c r="Q79" s="47">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="R79" s="36">
-        <f>SUM(L86:P86)</f>
-        <v>0</v>
-      </c>
+        <f t="shared" ref="L79" si="17">B79*$I79</f>
+        <v>0</v>
+      </c>
+      <c r="M79" s="49">
+        <f t="shared" ref="M79" si="18">C79*$I79</f>
+        <v>0</v>
+      </c>
+      <c r="N79" s="49">
+        <f t="shared" ref="N79" si="19">D79*$I79</f>
+        <v>0</v>
+      </c>
+      <c r="O79" s="49">
+        <f t="shared" ref="O79" si="20">E79*$I79</f>
+        <v>0</v>
+      </c>
+      <c r="P79" s="50">
+        <f t="shared" ref="P79:Q79" si="21">F79*$I79</f>
+        <v>0</v>
+      </c>
+      <c r="Q79" s="50">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="R79" s="36"/>
     </row>
     <row r="80" spans="1:18">
-      <c r="A80" s="42"/>
-      <c r="B80" s="43"/>
-      <c r="C80" s="43"/>
-      <c r="D80" s="43"/>
-      <c r="E80" s="43"/>
-      <c r="F80" s="43"/>
-      <c r="G80" s="43"/>
-      <c r="H80" s="43"/>
+      <c r="A80" s="44"/>
+      <c r="B80" s="38"/>
+      <c r="C80" s="38"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="38"/>
+      <c r="F80" s="38"/>
+      <c r="G80" s="38"/>
+      <c r="H80" s="38"/>
       <c r="I80" s="48"/>
-      <c r="J80" s="43"/>
-      <c r="K80" s="49"/>
+      <c r="J80" s="38"/>
+      <c r="K80" s="39"/>
       <c r="L80" s="35"/>
       <c r="M80" s="35"/>
       <c r="N80" s="35"/>
       <c r="O80" s="35"/>
       <c r="P80" s="34"/>
       <c r="Q80" s="34"/>
-      <c r="R80" s="36"/>
+      <c r="R80" s="36">
+        <f>SUM(L87:P87)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="81" spans="1:18">
       <c r="A81" s="15"/>
@@ -4740,200 +5019,321 @@
         <v>0</v>
       </c>
       <c r="M81">
-        <f t="shared" ref="M81" si="35">SUM(M79:M80)</f>
+        <f t="shared" ref="M81" si="22">SUM(M79:M80)</f>
         <v>0</v>
       </c>
       <c r="N81">
-        <f t="shared" ref="N81" si="36">SUM(N79:N80)</f>
+        <f t="shared" ref="N81" si="23">SUM(N79:N80)</f>
         <v>0</v>
       </c>
       <c r="O81">
-        <f t="shared" ref="O81" si="37">SUM(O79:O80)</f>
+        <f t="shared" ref="O81" si="24">SUM(O79:O80)</f>
         <v>0</v>
       </c>
       <c r="P81" s="36">
-        <f t="shared" ref="P81:Q81" si="38">SUM(P79:P80)</f>
+        <f t="shared" ref="P81:Q81" si="25">SUM(P79:P80)</f>
         <v>0</v>
       </c>
       <c r="Q81" s="36">
-        <f t="shared" si="38"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="R81" s="36"/>
     </row>
     <row r="82" spans="1:18">
       <c r="A82" s="15"/>
-      <c r="K82" t="s">
-        <v>122</v>
+      <c r="K82" s="35" t="s">
+        <v>63</v>
       </c>
       <c r="P82" s="36"/>
-      <c r="Q82" s="41"/>
-      <c r="R82" s="41">
-        <f>SUM(L89:Q89)</f>
-        <v>222</v>
-      </c>
-    </row>
-    <row r="83" spans="1:17">
-      <c r="A83" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="L83" s="31"/>
-      <c r="M83" s="11"/>
-      <c r="N83" s="11"/>
-      <c r="O83" s="11"/>
-      <c r="P83" s="32"/>
-      <c r="Q83" s="34"/>
-    </row>
-    <row r="84" spans="1:17">
-      <c r="A84" s="42"/>
-      <c r="B84" s="43"/>
-      <c r="C84" s="43"/>
-      <c r="D84" s="43"/>
-      <c r="E84" s="43"/>
-      <c r="F84" s="43"/>
-      <c r="G84" s="43"/>
-      <c r="H84" s="43"/>
-      <c r="I84" s="48"/>
-      <c r="J84" s="43"/>
-      <c r="K84" s="49"/>
-      <c r="L84" s="37">
-        <f t="shared" ref="L84" si="39">B84*$I84</f>
-        <v>0</v>
-      </c>
-      <c r="M84" s="46">
-        <f t="shared" ref="M84" si="40">C84*$I84</f>
-        <v>0</v>
-      </c>
-      <c r="N84" s="46">
-        <f t="shared" ref="N84" si="41">D84*$I84</f>
-        <v>0</v>
-      </c>
-      <c r="O84" s="46">
-        <f t="shared" ref="O84" si="42">E84*$I84</f>
-        <v>0</v>
-      </c>
-      <c r="P84" s="47">
-        <f t="shared" ref="P84:Q84" si="43">F84*$I84</f>
-        <v>0</v>
-      </c>
-      <c r="Q84" s="47">
-        <f t="shared" si="43"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:17">
-      <c r="A85" s="42"/>
-      <c r="B85" s="43"/>
-      <c r="C85" s="43"/>
-      <c r="D85" s="43"/>
-      <c r="E85" s="43"/>
-      <c r="F85" s="43"/>
-      <c r="G85" s="43"/>
-      <c r="H85" s="43"/>
+      <c r="Q82" s="36"/>
+      <c r="R82" s="36"/>
+    </row>
+    <row r="83" spans="1:18">
+      <c r="A83" s="15"/>
+      <c r="K83" s="35"/>
+      <c r="P83" s="36"/>
+      <c r="Q83" s="43"/>
+      <c r="R83" s="36"/>
+    </row>
+    <row r="84" spans="1:18">
+      <c r="A84" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="L84" s="31"/>
+      <c r="M84" s="11"/>
+      <c r="N84" s="11"/>
+      <c r="O84" s="11"/>
+      <c r="P84" s="32"/>
+      <c r="Q84" s="34"/>
+      <c r="R84" s="36"/>
+    </row>
+    <row r="85" spans="1:18">
+      <c r="A85" s="44"/>
+      <c r="B85" s="38"/>
+      <c r="C85" s="38"/>
+      <c r="D85" s="38"/>
+      <c r="E85" s="38"/>
+      <c r="F85" s="38"/>
+      <c r="G85" s="38"/>
+      <c r="H85" s="38"/>
       <c r="I85" s="48"/>
-      <c r="J85" s="43"/>
-      <c r="K85" s="49"/>
-      <c r="L85" s="35"/>
-      <c r="M85" s="35"/>
-      <c r="N85" s="35"/>
-      <c r="O85" s="35"/>
-      <c r="P85" s="34"/>
-      <c r="Q85" s="34"/>
-    </row>
-    <row r="86" spans="1:17">
-      <c r="A86" s="15"/>
-      <c r="H86" s="35"/>
-      <c r="K86" s="34" t="s">
+      <c r="J85" s="38"/>
+      <c r="K85" s="39"/>
+      <c r="L85" s="37">
+        <f t="shared" ref="L85" si="26">B85*$I85</f>
+        <v>0</v>
+      </c>
+      <c r="M85" s="49">
+        <f t="shared" ref="M85" si="27">C85*$I85</f>
+        <v>0</v>
+      </c>
+      <c r="N85" s="49">
+        <f t="shared" ref="N85" si="28">D85*$I85</f>
+        <v>0</v>
+      </c>
+      <c r="O85" s="49">
+        <f t="shared" ref="O85" si="29">E85*$I85</f>
+        <v>0</v>
+      </c>
+      <c r="P85" s="50">
+        <f t="shared" ref="P85:Q85" si="30">F85*$I85</f>
+        <v>0</v>
+      </c>
+      <c r="Q85" s="50">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="R85" s="36">
+        <f>SUM(L92:P92)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18">
+      <c r="A86" s="44"/>
+      <c r="B86" s="38"/>
+      <c r="C86" s="38"/>
+      <c r="D86" s="38"/>
+      <c r="E86" s="38"/>
+      <c r="F86" s="38"/>
+      <c r="G86" s="38"/>
+      <c r="H86" s="38"/>
+      <c r="I86" s="48"/>
+      <c r="J86" s="38"/>
+      <c r="K86" s="39"/>
+      <c r="L86" s="35"/>
+      <c r="M86" s="35"/>
+      <c r="N86" s="35"/>
+      <c r="O86" s="35"/>
+      <c r="P86" s="34"/>
+      <c r="Q86" s="34"/>
+      <c r="R86" s="36"/>
+    </row>
+    <row r="87" spans="1:18">
+      <c r="A87" s="15"/>
+      <c r="H87" s="35"/>
+      <c r="K87" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="L86">
-        <f>SUM(L84:L85)</f>
-        <v>0</v>
-      </c>
-      <c r="M86">
-        <f t="shared" ref="M86" si="44">SUM(M84:M85)</f>
-        <v>0</v>
-      </c>
-      <c r="N86">
-        <f t="shared" ref="N86" si="45">SUM(N84:N85)</f>
-        <v>0</v>
-      </c>
-      <c r="O86">
-        <f t="shared" ref="O86" si="46">SUM(O84:O85)</f>
-        <v>0</v>
-      </c>
-      <c r="P86" s="36">
-        <f t="shared" ref="P86:Q86" si="47">SUM(P84:P85)</f>
-        <v>0</v>
-      </c>
-      <c r="Q86" s="36">
-        <f t="shared" si="47"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:17">
-      <c r="A87" s="15"/>
-      <c r="K87" t="s">
-        <v>124</v>
-      </c>
-      <c r="P87" s="36"/>
-      <c r="Q87" s="36"/>
-    </row>
-    <row r="88" spans="1:17">
+      <c r="L87">
+        <f>SUM(L85:L86)</f>
+        <v>0</v>
+      </c>
+      <c r="M87">
+        <f t="shared" ref="M87" si="31">SUM(M85:M86)</f>
+        <v>0</v>
+      </c>
+      <c r="N87">
+        <f t="shared" ref="N87" si="32">SUM(N85:N86)</f>
+        <v>0</v>
+      </c>
+      <c r="O87">
+        <f t="shared" ref="O87" si="33">SUM(O85:O86)</f>
+        <v>0</v>
+      </c>
+      <c r="P87" s="36">
+        <f t="shared" ref="P87:Q87" si="34">SUM(P85:P86)</f>
+        <v>0</v>
+      </c>
+      <c r="Q87" s="36">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="R87" s="36"/>
+    </row>
+    <row r="88" spans="1:18">
       <c r="A88" s="15"/>
+      <c r="K88" t="s">
+        <v>135</v>
+      </c>
       <c r="P88" s="36"/>
-      <c r="Q88" s="36"/>
+      <c r="Q88" s="43"/>
+      <c r="R88" s="43">
+        <f>SUM(L95:Q95)</f>
+        <v>243</v>
+      </c>
     </row>
     <row r="89" spans="1:17">
-      <c r="A89" s="15"/>
-      <c r="K89" s="50" t="s">
-        <v>125</v>
-      </c>
-      <c r="L89">
-        <f>L34+L69+L75+L81+L86</f>
-        <v>46.5</v>
-      </c>
-      <c r="M89">
-        <f t="shared" ref="M89:Q89" si="48">M34+M69+M75+M81+M86</f>
-        <v>24.5</v>
-      </c>
-      <c r="N89">
-        <f t="shared" si="48"/>
-        <v>24.5</v>
-      </c>
-      <c r="O89">
-        <f t="shared" si="48"/>
-        <v>48.5</v>
-      </c>
-      <c r="P89" s="36">
-        <f t="shared" si="48"/>
-        <v>49</v>
-      </c>
-      <c r="Q89" s="36">
-        <f t="shared" si="48"/>
-        <v>29</v>
-      </c>
+      <c r="A89" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="L89" s="31"/>
+      <c r="M89" s="11"/>
+      <c r="N89" s="11"/>
+      <c r="O89" s="11"/>
+      <c r="P89" s="32"/>
+      <c r="Q89" s="34"/>
     </row>
     <row r="90" spans="1:17">
       <c r="A90" s="44"/>
-      <c r="B90" s="45"/>
-      <c r="C90" s="45"/>
-      <c r="D90" s="45"/>
-      <c r="E90" s="45"/>
-      <c r="F90" s="45"/>
-      <c r="G90" s="45"/>
-      <c r="H90" s="45"/>
-      <c r="I90" s="45"/>
-      <c r="J90" s="45"/>
-      <c r="K90" s="51" t="s">
-        <v>126</v>
-      </c>
-      <c r="L90" s="45"/>
-      <c r="M90" s="45"/>
-      <c r="N90" s="45"/>
-      <c r="O90" s="45"/>
-      <c r="P90" s="41"/>
-      <c r="Q90" s="41"/>
+      <c r="B90" s="38"/>
+      <c r="C90" s="38"/>
+      <c r="D90" s="38"/>
+      <c r="E90" s="38"/>
+      <c r="F90" s="38"/>
+      <c r="G90" s="38"/>
+      <c r="H90" s="38"/>
+      <c r="I90" s="48"/>
+      <c r="J90" s="38"/>
+      <c r="K90" s="39"/>
+      <c r="L90" s="37">
+        <f t="shared" ref="L90" si="35">B90*$I90</f>
+        <v>0</v>
+      </c>
+      <c r="M90" s="49">
+        <f t="shared" ref="M90" si="36">C90*$I90</f>
+        <v>0</v>
+      </c>
+      <c r="N90" s="49">
+        <f t="shared" ref="N90" si="37">D90*$I90</f>
+        <v>0</v>
+      </c>
+      <c r="O90" s="49">
+        <f t="shared" ref="O90" si="38">E90*$I90</f>
+        <v>0</v>
+      </c>
+      <c r="P90" s="50">
+        <f t="shared" ref="P90:Q90" si="39">F90*$I90</f>
+        <v>0</v>
+      </c>
+      <c r="Q90" s="50">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17">
+      <c r="A91" s="44"/>
+      <c r="B91" s="38"/>
+      <c r="C91" s="38"/>
+      <c r="D91" s="38"/>
+      <c r="E91" s="38"/>
+      <c r="F91" s="38"/>
+      <c r="G91" s="38"/>
+      <c r="H91" s="38"/>
+      <c r="I91" s="48"/>
+      <c r="J91" s="38"/>
+      <c r="K91" s="39"/>
+      <c r="L91" s="35"/>
+      <c r="M91" s="35"/>
+      <c r="N91" s="35"/>
+      <c r="O91" s="35"/>
+      <c r="P91" s="34"/>
+      <c r="Q91" s="34"/>
+    </row>
+    <row r="92" spans="1:17">
+      <c r="A92" s="15"/>
+      <c r="H92" s="35"/>
+      <c r="K92" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="L92">
+        <f>SUM(L90:L91)</f>
+        <v>0</v>
+      </c>
+      <c r="M92">
+        <f t="shared" ref="M92" si="40">SUM(M90:M91)</f>
+        <v>0</v>
+      </c>
+      <c r="N92">
+        <f t="shared" ref="N92" si="41">SUM(N90:N91)</f>
+        <v>0</v>
+      </c>
+      <c r="O92">
+        <f t="shared" ref="O92" si="42">SUM(O90:O91)</f>
+        <v>0</v>
+      </c>
+      <c r="P92" s="36">
+        <f t="shared" ref="P92:Q92" si="43">SUM(P90:P91)</f>
+        <v>0</v>
+      </c>
+      <c r="Q92" s="36">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17">
+      <c r="A93" s="15"/>
+      <c r="K93" t="s">
+        <v>137</v>
+      </c>
+      <c r="P93" s="36"/>
+      <c r="Q93" s="36"/>
+    </row>
+    <row r="94" spans="1:17">
+      <c r="A94" s="15"/>
+      <c r="P94" s="36"/>
+      <c r="Q94" s="36"/>
+    </row>
+    <row r="95" spans="1:17">
+      <c r="A95" s="15"/>
+      <c r="K95" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="L95">
+        <f>L34+L75+L81+L87+L92</f>
+        <v>46.5</v>
+      </c>
+      <c r="M95">
+        <f t="shared" ref="M95:Q95" si="44">M34+M75+M81+M87+M92</f>
+        <v>24.5</v>
+      </c>
+      <c r="N95">
+        <f t="shared" si="44"/>
+        <v>24.5</v>
+      </c>
+      <c r="O95">
+        <f t="shared" si="44"/>
+        <v>48.5</v>
+      </c>
+      <c r="P95" s="36">
+        <f t="shared" si="44"/>
+        <v>51</v>
+      </c>
+      <c r="Q95" s="36">
+        <f t="shared" si="44"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17">
+      <c r="A96" s="45"/>
+      <c r="B96" s="46"/>
+      <c r="C96" s="46"/>
+      <c r="D96" s="46"/>
+      <c r="E96" s="46"/>
+      <c r="F96" s="46"/>
+      <c r="G96" s="46"/>
+      <c r="H96" s="46"/>
+      <c r="I96" s="46"/>
+      <c r="J96" s="46"/>
+      <c r="K96" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="L96" s="46"/>
+      <c r="M96" s="46"/>
+      <c r="N96" s="46"/>
+      <c r="O96" s="46"/>
+      <c r="P96" s="43"/>
+      <c r="Q96" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>